<commit_message>
updated survey code for new va estimates
</commit_message>
<xml_diff>
--- a/out/csv/factoranalysis/alpha.xlsx
+++ b/out/csv/factoranalysis/alpha.xlsx
@@ -1374,7 +1374,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>0.95354200195643479</v>
+        <v>0.93811986667109926</v>
       </c>
     </row>
     <row r="4">
@@ -1399,16 +1399,16 @@
         <v>73</v>
       </c>
       <c r="B5">
-        <v>0.61622277865838992</v>
+        <v>0.52021457595164078</v>
       </c>
       <c r="C5">
-        <v>0.56601003818575979</v>
+        <v>0.46088335413329407</v>
       </c>
       <c r="D5">
-        <v>0.51409341062060721</v>
+        <v>0.44208830353793116</v>
       </c>
       <c r="E5">
-        <v>0.95261149914431831</v>
+        <v>0.93771631321975168</v>
       </c>
     </row>
     <row r="6">
@@ -1416,16 +1416,16 @@
         <v>74</v>
       </c>
       <c r="B6">
-        <v>0.62635615506399211</v>
+        <v>0.59109636684383315</v>
       </c>
       <c r="C6">
-        <v>0.57897423925374525</v>
+        <v>0.5386377017423325</v>
       </c>
       <c r="D6">
-        <v>0.51372573458784987</v>
+        <v>0.43751734969827177</v>
       </c>
       <c r="E6">
-        <v>0.95254501169266181</v>
+        <v>0.93662390329116285</v>
       </c>
     </row>
     <row r="7">
@@ -1433,16 +1433,16 @@
         <v>75</v>
       </c>
       <c r="B7">
-        <v>0.5295325712521739</v>
+        <v>0.47311259405578543</v>
       </c>
       <c r="C7">
-        <v>0.47338017871049132</v>
+        <v>0.41138034118202949</v>
       </c>
       <c r="D7">
-        <v>0.51967362368938841</v>
+        <v>0.44551708765766174</v>
       </c>
       <c r="E7">
-        <v>0.95361014418818291</v>
+        <v>0.93852267399053968</v>
       </c>
     </row>
     <row r="8">
@@ -1450,16 +1450,16 @@
         <v>76</v>
       </c>
       <c r="B8">
-        <v>0.5838690331943851</v>
+        <v>0.54685124704182164</v>
       </c>
       <c r="C8">
-        <v>0.53209123447069884</v>
+        <v>0.49043465758161364</v>
       </c>
       <c r="D8">
-        <v>0.51629226808833084</v>
+        <v>0.44049910582768553</v>
       </c>
       <c r="E8">
-        <v>0.95300733750871935</v>
+        <v>0.93733879463424963</v>
       </c>
     </row>
     <row r="9">
@@ -1467,16 +1467,16 @@
         <v>77</v>
       </c>
       <c r="B9">
-        <v>0.55912618543730475</v>
+        <v>0.53862495167377233</v>
       </c>
       <c r="C9">
-        <v>0.47617739645811547</v>
+        <v>0.47094554250875525</v>
       </c>
       <c r="D9">
-        <v>0.52570680395459057</v>
+        <v>0.44396287469296303</v>
       </c>
       <c r="E9">
-        <v>0.95466828090377531</v>
+        <v>0.93815853523046633</v>
       </c>
     </row>
     <row r="10">
@@ -1484,16 +1484,16 @@
         <v>78</v>
       </c>
       <c r="B10">
-        <v>0.80825681497040447</v>
+        <v>0.78476474115159434</v>
       </c>
       <c r="C10">
-        <v>0.76854100153974758</v>
+        <v>0.74717071260263157</v>
       </c>
       <c r="D10">
-        <v>0.49818887097816833</v>
+        <v>0.42142270881698352</v>
       </c>
       <c r="E10">
-        <v>0.94965475999229665</v>
+        <v>0.93261080169809207</v>
       </c>
     </row>
     <row r="11">
@@ -1501,16 +1501,16 @@
         <v>79</v>
       </c>
       <c r="B11">
-        <v>0.84221423336576395</v>
+        <v>0.8152789509224877</v>
       </c>
       <c r="C11">
-        <v>0.81050861716693967</v>
+        <v>0.78282266201245565</v>
       </c>
       <c r="D11">
-        <v>0.49450395817522735</v>
+        <v>0.41841427076689441</v>
       </c>
       <c r="E11">
-        <v>0.94894531821795847</v>
+        <v>0.93183043203103233</v>
       </c>
     </row>
     <row r="12">
@@ -1518,16 +1518,16 @@
         <v>80</v>
       </c>
       <c r="B12">
-        <v>0.81452611277490694</v>
+        <v>0.76951665233257049</v>
       </c>
       <c r="C12">
-        <v>0.774581894548104</v>
+        <v>0.72910967655718306</v>
       </c>
       <c r="D12">
-        <v>0.49707801051184014</v>
+        <v>0.42290307380571585</v>
       </c>
       <c r="E12">
-        <v>0.94944188655433104</v>
+        <v>0.93299119636126671</v>
       </c>
     </row>
     <row r="13">
@@ -1535,16 +1535,16 @@
         <v>81</v>
       </c>
       <c r="B13">
-        <v>0.83572260750981686</v>
+        <v>0.84021421332046153</v>
       </c>
       <c r="C13">
-        <v>0.79845945872119883</v>
+        <v>0.8086126296609738</v>
       </c>
       <c r="D13">
-        <v>0.49383496601182453</v>
+        <v>0.41630576233609057</v>
       </c>
       <c r="E13">
-        <v>0.9488154990628811</v>
+        <v>0.93127756733082889</v>
       </c>
     </row>
     <row r="14">
@@ -1552,16 +1552,16 @@
         <v>82</v>
       </c>
       <c r="B14">
-        <v>0.78956051368233604</v>
+        <v>0.7378263487386848</v>
       </c>
       <c r="C14">
-        <v>0.74597092702953727</v>
+        <v>0.69203546312319986</v>
       </c>
       <c r="D14">
-        <v>0.49820353425096131</v>
+        <v>0.42589317955654699</v>
       </c>
       <c r="E14">
-        <v>0.94965756419412906</v>
+        <v>0.93375239972217805</v>
       </c>
     </row>
     <row r="15">
@@ -1569,16 +1569,16 @@
         <v>83</v>
       </c>
       <c r="B15">
-        <v>0.77277435358654867</v>
+        <v>0.76890380732505403</v>
       </c>
       <c r="C15">
-        <v>0.72373253077747535</v>
+        <v>0.72755326672862342</v>
       </c>
       <c r="D15">
-        <v>0.50083786576738409</v>
+        <v>0.42282378705797896</v>
       </c>
       <c r="E15">
-        <v>0.95015895476683931</v>
+        <v>0.93297088250453564</v>
       </c>
     </row>
     <row r="16">
@@ -1586,16 +1586,16 @@
         <v>84</v>
       </c>
       <c r="B16">
-        <v>0.85563562633025569</v>
+        <v>0.82498666731825854</v>
       </c>
       <c r="C16">
-        <v>0.82362592700678061</v>
+        <v>0.7943687624796536</v>
       </c>
       <c r="D16">
-        <v>0.49215966900972818</v>
+        <v>0.41755781209995524</v>
       </c>
       <c r="E16">
-        <v>0.94848901316541911</v>
+        <v>0.93160645726809987</v>
       </c>
     </row>
     <row r="17">
@@ -1603,16 +1603,16 @@
         <v>85</v>
       </c>
       <c r="B17">
-        <v>0.84928000853230001</v>
+        <v>0.81360892089385817</v>
       </c>
       <c r="C17">
-        <v>0.81676388591148119</v>
+        <v>0.78035305157606061</v>
       </c>
       <c r="D17">
-        <v>0.49329590396437489</v>
+        <v>0.41942866849568017</v>
       </c>
       <c r="E17">
-        <v>0.94871066284098582</v>
+        <v>0.9320946649843429</v>
       </c>
     </row>
     <row r="18">
@@ -1620,16 +1620,16 @@
         <v>86</v>
       </c>
       <c r="B18">
-        <v>0.52070599543445872</v>
+        <v>0.26596340886531933</v>
       </c>
       <c r="C18">
-        <v>0.45732783833370744</v>
+        <v>0.18794090417335127</v>
       </c>
       <c r="D18">
-        <v>0.52541181599548425</v>
+        <v>0.46422552969655684</v>
       </c>
       <c r="E18">
-        <v>0.95461705508162631</v>
+        <v>0.94273502981403401</v>
       </c>
     </row>
     <row r="19">
@@ -1637,16 +1637,16 @@
         <v>87</v>
       </c>
       <c r="B19">
-        <v>0.68903591568770428</v>
+        <v>0.65976071460772967</v>
       </c>
       <c r="C19">
-        <v>0.64535821090026058</v>
+        <v>0.61335628927590491</v>
       </c>
       <c r="D19">
-        <v>0.50910512287265819</v>
+        <v>0.43222507541203486</v>
       </c>
       <c r="E19">
-        <v>0.95170207761925341</v>
+        <v>0.93533353035476741</v>
       </c>
     </row>
     <row r="20">
@@ -1654,16 +1654,16 @@
         <v>88</v>
       </c>
       <c r="B20">
-        <v>0.68221212285697841</v>
+        <v>0.61033157636876678</v>
       </c>
       <c r="C20">
-        <v>0.63324654157250093</v>
+        <v>0.55488810277002099</v>
       </c>
       <c r="D20">
-        <v>0.51025658789422734</v>
+        <v>0.43672983408746191</v>
       </c>
       <c r="E20">
-        <v>0.95191342629495124</v>
+        <v>0.93643364671490026</v>
       </c>
     </row>
     <row r="21">
@@ -1671,16 +1671,16 @@
         <v>89</v>
       </c>
       <c r="B21">
-        <v>0.781217350249786</v>
+        <v>0.74332002454423496</v>
       </c>
       <c r="C21">
-        <v>0.74456362398457299</v>
+        <v>0.70281443410571387</v>
       </c>
       <c r="D21">
-        <v>0.50326573649606376</v>
+        <v>0.42658145967339672</v>
       </c>
       <c r="E21">
-        <v>0.95061686380788113</v>
+        <v>0.93392628118674414</v>
       </c>
     </row>
     <row r="22">
@@ -1688,16 +1688,16 @@
         <v>90</v>
       </c>
       <c r="B22">
-        <v>0.78208494830936548</v>
+        <v>0.75955882160231458</v>
       </c>
       <c r="C22">
-        <v>0.75082226159882293</v>
+        <v>0.724805030149963</v>
       </c>
       <c r="D22">
-        <v>0.50322007423518667</v>
+        <v>0.42606529162018753</v>
       </c>
       <c r="E22">
-        <v>0.95060828838393063</v>
+        <v>0.93379592730747929</v>
       </c>
     </row>
     <row r="23">
@@ -1705,16 +1705,16 @@
         <v>91</v>
       </c>
       <c r="B23">
-        <v>0.70732326990456829</v>
+        <v>0.67642171967914766</v>
       </c>
       <c r="C23">
-        <v>0.66420108393942157</v>
+        <v>0.62971163322889856</v>
       </c>
       <c r="D23">
-        <v>0.50881940952871518</v>
+        <v>0.43162552827468886</v>
       </c>
       <c r="E23">
-        <v>0.9516495020687824</v>
+        <v>0.93518557967801208</v>
       </c>
     </row>
     <row r="24">
@@ -1722,16 +1722,16 @@
         <v>92</v>
       </c>
       <c r="B24">
-        <v>0.70413908606887388</v>
+        <v>0.69513450010582534</v>
       </c>
       <c r="C24">
-        <v>0.65879241059588534</v>
+        <v>0.64966957057701935</v>
       </c>
       <c r="D24">
-        <v>0.50901463390407731</v>
+        <v>0.43047783149984775</v>
       </c>
       <c r="E24">
-        <v>0.95168543204660816</v>
+        <v>0.93490134358069532</v>
       </c>
     </row>
   </sheetData>
@@ -1753,7 +1753,7 @@
         <v>94</v>
       </c>
       <c r="B2">
-        <v>0.9247487414744493</v>
+        <v>0.89980548376827996</v>
       </c>
     </row>
     <row r="4">
@@ -1778,16 +1778,16 @@
         <v>100</v>
       </c>
       <c r="B5">
-        <v>0.64125369414699862</v>
+        <v>0.60765057404749367</v>
       </c>
       <c r="C5">
-        <v>0.58078303011792987</v>
+        <v>0.54099130370298742</v>
       </c>
       <c r="D5">
-        <v>0.42421858555950592</v>
+        <v>0.34711186131012206</v>
       </c>
       <c r="E5">
-        <v>0.921803665000552</v>
+        <v>0.89480876128231535</v>
       </c>
     </row>
     <row r="6">
@@ -1795,16 +1795,16 @@
         <v>101</v>
       </c>
       <c r="B6">
-        <v>0.578906110778448</v>
+        <v>0.57890901691872954</v>
       </c>
       <c r="C6">
-        <v>0.50822983151971723</v>
+        <v>0.50613589588786334</v>
       </c>
       <c r="D6">
-        <v>0.42879528937709621</v>
+        <v>0.34931225267703742</v>
       </c>
       <c r="E6">
-        <v>0.92314180013820601</v>
+        <v>0.89571783295340035</v>
       </c>
     </row>
     <row r="7">
@@ -1812,16 +1812,16 @@
         <v>102</v>
       </c>
       <c r="B7">
-        <v>0.68946437102777092</v>
+        <v>0.5704209036028508</v>
       </c>
       <c r="C7">
-        <v>0.63588247277771148</v>
+        <v>0.50065923643525823</v>
       </c>
       <c r="D7">
-        <v>0.42037789339415355</v>
+        <v>0.34918428976873922</v>
       </c>
       <c r="E7">
-        <v>0.92066131737741264</v>
+        <v>0.89566522970794993</v>
       </c>
     </row>
     <row r="8">
@@ -1829,16 +1829,16 @@
         <v>103</v>
       </c>
       <c r="B8">
-        <v>0.61737211611832377</v>
+        <v>0.53503182891015633</v>
       </c>
       <c r="C8">
-        <v>0.54873299469866932</v>
+        <v>0.45733791410152069</v>
       </c>
       <c r="D8">
-        <v>0.42539511455665541</v>
+        <v>0.35260948418173588</v>
       </c>
       <c r="E8">
-        <v>0.92215003516905125</v>
+        <v>0.89706219246221153</v>
       </c>
     </row>
     <row r="9">
@@ -1846,16 +1846,16 @@
         <v>104</v>
       </c>
       <c r="B9">
-        <v>0.63821233945550027</v>
+        <v>0.54932073727996222</v>
       </c>
       <c r="C9">
-        <v>0.57581973020334332</v>
+        <v>0.47584282472940015</v>
       </c>
       <c r="D9">
-        <v>0.42493460770030289</v>
+        <v>0.35127111453286131</v>
       </c>
       <c r="E9">
-        <v>0.92201465940187621</v>
+        <v>0.89651906501406109</v>
       </c>
     </row>
     <row r="10">
@@ -1863,16 +1863,16 @@
         <v>105</v>
       </c>
       <c r="B10">
-        <v>0.83146063115912128</v>
+        <v>0.76272895271912244</v>
       </c>
       <c r="C10">
-        <v>0.79212119935854253</v>
+        <v>0.7117936217212274</v>
       </c>
       <c r="D10">
-        <v>0.39831324027633319</v>
+        <v>0.33088834881486806</v>
       </c>
       <c r="E10">
-        <v>0.91373293759731922</v>
+        <v>0.88779554608734645</v>
       </c>
     </row>
     <row r="11">
@@ -1880,16 +1880,16 @@
         <v>106</v>
       </c>
       <c r="B11">
-        <v>0.85250866749033627</v>
+        <v>0.79083360931839053</v>
       </c>
       <c r="C11">
-        <v>0.8180484400322513</v>
+        <v>0.74635828466019827</v>
       </c>
       <c r="D11">
-        <v>0.39626434479673533</v>
+        <v>0.3283942465983597</v>
       </c>
       <c r="E11">
-        <v>0.91305606519428517</v>
+        <v>0.88666629527227803</v>
       </c>
     </row>
     <row r="12">
@@ -1897,16 +1897,16 @@
         <v>107</v>
       </c>
       <c r="B12">
-        <v>0.79184229848676724</v>
+        <v>0.74898648072644181</v>
       </c>
       <c r="C12">
-        <v>0.74081413876354929</v>
+        <v>0.69562621214810938</v>
       </c>
       <c r="D12">
-        <v>0.40457815880986708</v>
+        <v>0.33254915084140568</v>
       </c>
       <c r="E12">
-        <v>0.91576610019529614</v>
+        <v>0.88853967872568107</v>
       </c>
     </row>
     <row r="13">
@@ -1914,16 +1914,16 @@
         <v>108</v>
       </c>
       <c r="B13">
-        <v>0.85292946597115149</v>
+        <v>0.73765275982885248</v>
       </c>
       <c r="C13">
-        <v>0.81735243999561524</v>
+        <v>0.68385891674021859</v>
       </c>
       <c r="D13">
-        <v>0.39573442927430269</v>
+        <v>0.33440865992823343</v>
       </c>
       <c r="E13">
-        <v>0.91288002616054365</v>
+        <v>0.88936553045657074</v>
       </c>
     </row>
     <row r="14">
@@ -1931,16 +1931,16 @@
         <v>109</v>
       </c>
       <c r="B14">
-        <v>0.84127737568125094</v>
+        <v>0.77405707165228466</v>
       </c>
       <c r="C14">
-        <v>0.80103089028242869</v>
+        <v>0.72439603017699539</v>
       </c>
       <c r="D14">
-        <v>0.39689615018130819</v>
+        <v>0.32982355817976178</v>
       </c>
       <c r="E14">
-        <v>0.91326542625951823</v>
+        <v>0.8873151804133691</v>
       </c>
     </row>
     <row r="15">
@@ -1948,16 +1948,16 @@
         <v>110</v>
       </c>
       <c r="B15">
-        <v>0.81273660960793837</v>
+        <v>0.7321382045732433</v>
       </c>
       <c r="C15">
-        <v>0.76697454065180704</v>
+        <v>0.6767540676300533</v>
       </c>
       <c r="D15">
-        <v>0.40231753388413377</v>
+        <v>0.33478932057131988</v>
       </c>
       <c r="E15">
-        <v>0.91503872050644552</v>
+        <v>0.88953364742748453</v>
       </c>
     </row>
     <row r="16">
@@ -1965,16 +1965,16 @@
         <v>111</v>
       </c>
       <c r="B16">
-        <v>0.4439015622325731</v>
+        <v>0.44061752009594934</v>
       </c>
       <c r="C16">
-        <v>0.35174535929109779</v>
+        <v>0.34975492578928696</v>
       </c>
       <c r="D16">
-        <v>0.44597039050765863</v>
+        <v>0.36286363371859487</v>
       </c>
       <c r="E16">
-        <v>0.9279503758407982</v>
+        <v>0.90111114928563685</v>
       </c>
     </row>
     <row r="17">
@@ -1982,16 +1982,16 @@
         <v>112</v>
       </c>
       <c r="B17">
-        <v>0.50869390829294114</v>
+        <v>0.47620613915187499</v>
       </c>
       <c r="C17">
-        <v>0.42555086460274821</v>
+        <v>0.38898181168285684</v>
       </c>
       <c r="D17">
-        <v>0.44049637232144201</v>
+        <v>0.35988615307866706</v>
       </c>
       <c r="E17">
-        <v>0.92645315415796337</v>
+        <v>0.89995551667692608</v>
       </c>
     </row>
     <row r="18">
@@ -1999,16 +1999,16 @@
         <v>113</v>
       </c>
       <c r="B18">
-        <v>0.62708155017997402</v>
+        <v>0.55467051167483483</v>
       </c>
       <c r="C18">
-        <v>0.55764499458715067</v>
+        <v>0.47558276939538946</v>
       </c>
       <c r="D18">
-        <v>0.42794258575335331</v>
+        <v>0.35284101886260411</v>
       </c>
       <c r="E18">
-        <v>0.92289436405975167</v>
+        <v>0.89715580056323885</v>
       </c>
     </row>
     <row r="19">
@@ -2016,16 +2016,16 @@
         <v>114</v>
       </c>
       <c r="B19">
-        <v>0.58234954730035393</v>
+        <v>0.52646442951524608</v>
       </c>
       <c r="C19">
-        <v>0.50762294593370227</v>
+        <v>0.44420698421811888</v>
       </c>
       <c r="D19">
-        <v>0.43395371891414813</v>
+        <v>0.35552601201254852</v>
       </c>
       <c r="E19">
-        <v>0.9246206909946838</v>
+        <v>0.89823382852846245</v>
       </c>
     </row>
     <row r="20">
@@ -2033,16 +2033,16 @@
         <v>115</v>
       </c>
       <c r="B20">
-        <v>0.49392954724074045</v>
+        <v>0.49350866726822967</v>
       </c>
       <c r="C20">
-        <v>0.40899382096534798</v>
+        <v>0.40812797146854823</v>
       </c>
       <c r="D20">
-        <v>0.44051294071945174</v>
+        <v>0.35838494836191814</v>
       </c>
       <c r="E20">
-        <v>0.92645773461279202</v>
+        <v>0.89936672332607048</v>
       </c>
     </row>
     <row r="21">
@@ -2050,16 +2050,16 @@
         <v>116</v>
       </c>
       <c r="B21">
-        <v>0.68937963192354956</v>
+        <v>0.64001003189013472</v>
       </c>
       <c r="C21">
-        <v>0.62757832744398756</v>
+        <v>0.57090761410195578</v>
       </c>
       <c r="D21">
-        <v>0.42155384088557901</v>
+        <v>0.34507033591622038</v>
       </c>
       <c r="E21">
-        <v>0.92101299171631379</v>
+        <v>0.8939566341337134</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2081,7 @@
         <v>118</v>
       </c>
       <c r="B2">
-        <v>0.7098361624622439</v>
+        <v>0.66211117647631301</v>
       </c>
     </row>
     <row r="4">
@@ -2106,16 +2106,16 @@
         <v>124</v>
       </c>
       <c r="B5">
-        <v>0.77463890660688228</v>
+        <v>0.72440688132534969</v>
       </c>
       <c r="C5">
-        <v>0.53057130121191687</v>
+        <v>0.45125479042373434</v>
       </c>
       <c r="D5">
-        <v>0.36854272938341653</v>
+        <v>0.31803270388592036</v>
       </c>
       <c r="E5">
-        <v>0.63648462576800424</v>
+        <v>0.58316623964145087</v>
       </c>
     </row>
     <row r="6">
@@ -2123,16 +2123,16 @@
         <v>125</v>
       </c>
       <c r="B6">
-        <v>0.73586292627178185</v>
+        <v>0.64920938872831568</v>
       </c>
       <c r="C6">
-        <v>0.46986011161090091</v>
+        <v>0.34990273077469564</v>
       </c>
       <c r="D6">
-        <v>0.40658434640046731</v>
+        <v>0.38755529935631444</v>
       </c>
       <c r="E6">
-        <v>0.67271900515619432</v>
+        <v>0.65498222979015974</v>
       </c>
     </row>
     <row r="7">
@@ -2140,16 +2140,16 @@
         <v>126</v>
       </c>
       <c r="B7">
-        <v>0.81636394341574559</v>
+        <v>0.76412230331561881</v>
       </c>
       <c r="C7">
-        <v>0.50207235886458124</v>
+        <v>0.46341058296824783</v>
       </c>
       <c r="D7">
-        <v>0.37444270781046057</v>
+        <v>0.29898614071388335</v>
       </c>
       <c r="E7">
-        <v>0.6423108760573415</v>
+        <v>0.56131037600992029</v>
       </c>
     </row>
     <row r="8">
@@ -2157,16 +2157,16 @@
         <v>127</v>
       </c>
       <c r="B8">
-        <v>0.78836031189541755</v>
+        <v>0.74125341506934572</v>
       </c>
       <c r="C8">
-        <v>0.50001282488222698</v>
+        <v>0.46009249225466198</v>
       </c>
       <c r="D8">
-        <v>0.3660177430452653</v>
+        <v>0.30776620003126054</v>
       </c>
       <c r="E8">
-        <v>0.63396693540862148</v>
+        <v>0.57151351471381817</v>
       </c>
     </row>
   </sheetData>
@@ -2188,7 +2188,7 @@
         <v>129</v>
       </c>
       <c r="B2">
-        <v>0.91366528184120499</v>
+        <v>0.94879129730325307</v>
       </c>
     </row>
     <row r="4">
@@ -2213,16 +2213,16 @@
         <v>135</v>
       </c>
       <c r="B5">
-        <v>0.86556172120234376</v>
+        <v>0.93251077638388924</v>
       </c>
       <c r="C5">
-        <v>0.75968486614984743</v>
+        <v>0.87853374268790541</v>
       </c>
       <c r="D5">
-        <v>0.75619805075894075</v>
+        <v>0.82029816548400292</v>
       </c>
       <c r="E5">
-        <v>0.90296038546877044</v>
+        <v>0.93194649541525321</v>
       </c>
     </row>
     <row r="6">
@@ -2230,16 +2230,16 @@
         <v>136</v>
       </c>
       <c r="B6">
-        <v>0.80388791371431412</v>
+        <v>0.87021774315021971</v>
       </c>
       <c r="C6">
-        <v>0.66060471063911319</v>
+        <v>0.77377575858429226</v>
       </c>
       <c r="D6">
-        <v>0.82948487527306669</v>
+        <v>0.89889402367670834</v>
       </c>
       <c r="E6">
-        <v>0.93587173201503659</v>
+        <v>0.96386217447067379</v>
       </c>
     </row>
     <row r="7">
@@ -2247,16 +2247,16 @@
         <v>137</v>
       </c>
       <c r="B7">
-        <v>0.96491834785607866</v>
+        <v>0.96807253793751136</v>
       </c>
       <c r="C7">
-        <v>0.933657217301611</v>
+        <v>0.94150521098901219</v>
       </c>
       <c r="D7">
-        <v>0.63813282660302173</v>
+        <v>0.77628584993049388</v>
       </c>
       <c r="E7">
-        <v>0.84102594840487943</v>
+        <v>0.91235734922482714</v>
       </c>
     </row>
     <row r="8">
@@ -2264,16 +2264,16 @@
         <v>138</v>
       </c>
       <c r="B8">
-        <v>0.93052428389223785</v>
+        <v>0.95472308681019069</v>
       </c>
       <c r="C8">
-        <v>0.87123222374875953</v>
+        <v>0.9170570109632542</v>
       </c>
       <c r="D8">
-        <v>0.67900320500755285</v>
+        <v>0.79430254063074579</v>
       </c>
       <c r="E8">
-        <v>0.8638694137432853</v>
+        <v>0.92053733462154352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug for running whole project
</commit_message>
<xml_diff>
--- a/out/csv/factoranalysis/alpha.xlsx
+++ b/out/csv/factoranalysis/alpha.xlsx
@@ -1374,7 +1374,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>0.93811986667109926</v>
+        <v>0.93476056157324883</v>
       </c>
     </row>
     <row r="4">
@@ -1399,16 +1399,16 @@
         <v>73</v>
       </c>
       <c r="B5">
-        <v>0.52021457595164078</v>
+        <v>0.52373588132351678</v>
       </c>
       <c r="C5">
-        <v>0.46088335413329407</v>
+        <v>0.46357909123400726</v>
       </c>
       <c r="D5">
-        <v>0.44208830353793116</v>
+        <v>0.42846196583932128</v>
       </c>
       <c r="E5">
-        <v>0.93771631321975168</v>
+        <v>0.93439883556814018</v>
       </c>
     </row>
     <row r="6">
@@ -1416,16 +1416,16 @@
         <v>74</v>
       </c>
       <c r="B6">
-        <v>0.59109636684383315</v>
+        <v>0.59251316719084646</v>
       </c>
       <c r="C6">
-        <v>0.5386377017423325</v>
+        <v>0.53891351314369262</v>
       </c>
       <c r="D6">
-        <v>0.43751734969827177</v>
+        <v>0.42333952995152985</v>
       </c>
       <c r="E6">
-        <v>0.93662390329116285</v>
+        <v>0.93310289925705125</v>
       </c>
     </row>
     <row r="7">
@@ -1433,16 +1433,16 @@
         <v>75</v>
       </c>
       <c r="B7">
-        <v>0.47311259405578543</v>
+        <v>0.47399432214396608</v>
       </c>
       <c r="C7">
-        <v>0.41138034118202949</v>
+        <v>0.41091850756826753</v>
       </c>
       <c r="D7">
-        <v>0.44551708765766174</v>
+        <v>0.43250728611586581</v>
       </c>
       <c r="E7">
-        <v>0.93852267399053968</v>
+        <v>0.93540304587500611</v>
       </c>
     </row>
     <row r="8">
@@ -1450,16 +1450,16 @@
         <v>76</v>
       </c>
       <c r="B8">
-        <v>0.54685124704182164</v>
+        <v>0.54909354335020133</v>
       </c>
       <c r="C8">
-        <v>0.49043465758161364</v>
+        <v>0.49152066719861881</v>
       </c>
       <c r="D8">
-        <v>0.44049910582768553</v>
+        <v>0.4267227188967791</v>
       </c>
       <c r="E8">
-        <v>0.93733879463424963</v>
+        <v>0.93396190638022281</v>
       </c>
     </row>
     <row r="9">
@@ -1467,16 +1467,16 @@
         <v>77</v>
       </c>
       <c r="B9">
-        <v>0.53862495167377233</v>
+        <v>0.51890870989776039</v>
       </c>
       <c r="C9">
-        <v>0.47094554250875525</v>
+        <v>0.45715157956819463</v>
       </c>
       <c r="D9">
-        <v>0.44396287469296303</v>
+        <v>0.42996012074238438</v>
       </c>
       <c r="E9">
-        <v>0.93815853523046633</v>
+        <v>0.93477268865455765</v>
       </c>
     </row>
     <row r="10">
@@ -1484,16 +1484,16 @@
         <v>78</v>
       </c>
       <c r="B10">
-        <v>0.78476474115159434</v>
+        <v>0.77090251752710426</v>
       </c>
       <c r="C10">
-        <v>0.74717071260263157</v>
+        <v>0.73492784796474975</v>
       </c>
       <c r="D10">
-        <v>0.42142270881698352</v>
+        <v>0.40927159241640076</v>
       </c>
       <c r="E10">
-        <v>0.93261080169809207</v>
+        <v>0.92939688439252799</v>
       </c>
     </row>
     <row r="11">
@@ -1501,16 +1501,16 @@
         <v>79</v>
       </c>
       <c r="B11">
-        <v>0.8152789509224877</v>
+        <v>0.80061650505030113</v>
       </c>
       <c r="C11">
-        <v>0.78282266201245565</v>
+        <v>0.76826267875016951</v>
       </c>
       <c r="D11">
-        <v>0.41841427076689441</v>
+        <v>0.40673690572357024</v>
       </c>
       <c r="E11">
-        <v>0.93183043203103233</v>
+        <v>0.92870517355628091</v>
       </c>
     </row>
     <row r="12">
@@ -1518,16 +1518,16 @@
         <v>80</v>
       </c>
       <c r="B12">
-        <v>0.76951665233257049</v>
+        <v>0.75210045074974896</v>
       </c>
       <c r="C12">
-        <v>0.72910967655718306</v>
+        <v>0.71299111933680426</v>
       </c>
       <c r="D12">
-        <v>0.42290307380571585</v>
+        <v>0.41044119372959637</v>
       </c>
       <c r="E12">
-        <v>0.93299119636126671</v>
+        <v>0.92971352897790249</v>
       </c>
     </row>
     <row r="13">
@@ -1535,16 +1535,16 @@
         <v>81</v>
       </c>
       <c r="B13">
-        <v>0.84021421332046153</v>
+        <v>0.83990682197243183</v>
       </c>
       <c r="C13">
-        <v>0.8086126296609738</v>
+        <v>0.81318604897136504</v>
       </c>
       <c r="D13">
-        <v>0.41630576233609057</v>
+        <v>0.40355781856995915</v>
       </c>
       <c r="E13">
-        <v>0.93127756733082889</v>
+        <v>0.92782681007882262</v>
       </c>
     </row>
     <row r="14">
@@ -1552,16 +1552,16 @@
         <v>82</v>
       </c>
       <c r="B14">
-        <v>0.7378263487386848</v>
+        <v>0.73539096330184228</v>
       </c>
       <c r="C14">
-        <v>0.69203546312319986</v>
+        <v>0.69614789143724476</v>
       </c>
       <c r="D14">
-        <v>0.42589317955654699</v>
+        <v>0.41199258273379419</v>
       </c>
       <c r="E14">
-        <v>0.93375239972217805</v>
+        <v>0.93013109012361239</v>
       </c>
     </row>
     <row r="15">
@@ -1569,16 +1569,16 @@
         <v>83</v>
       </c>
       <c r="B15">
-        <v>0.76890380732505403</v>
+        <v>0.76595155849930652</v>
       </c>
       <c r="C15">
-        <v>0.72755326672862342</v>
+        <v>0.72982799609508942</v>
       </c>
       <c r="D15">
-        <v>0.42282378705797896</v>
+        <v>0.40952865767137958</v>
       </c>
       <c r="E15">
-        <v>0.93297088250453564</v>
+        <v>0.92946661587351143</v>
       </c>
     </row>
     <row r="16">
@@ -1586,16 +1586,16 @@
         <v>84</v>
       </c>
       <c r="B16">
-        <v>0.82498666731825854</v>
+        <v>0.81908087946792407</v>
       </c>
       <c r="C16">
-        <v>0.7943687624796536</v>
+        <v>0.79026917878875036</v>
       </c>
       <c r="D16">
-        <v>0.41755781209995524</v>
+        <v>0.40533097345384811</v>
       </c>
       <c r="E16">
-        <v>0.93160645726809987</v>
+        <v>0.92831821704040562</v>
       </c>
     </row>
     <row r="17">
@@ -1603,16 +1603,16 @@
         <v>85</v>
       </c>
       <c r="B17">
-        <v>0.81360892089385817</v>
+        <v>0.79621466286102838</v>
       </c>
       <c r="C17">
-        <v>0.78035305157606061</v>
+        <v>0.76417205183184378</v>
       </c>
       <c r="D17">
-        <v>0.41942866849568017</v>
+        <v>0.40721760749368463</v>
       </c>
       <c r="E17">
-        <v>0.9320946649843429</v>
+        <v>0.92883693833443903</v>
       </c>
     </row>
     <row r="18">
@@ -1620,16 +1620,16 @@
         <v>86</v>
       </c>
       <c r="B18">
-        <v>0.26596340886531933</v>
+        <v>0.27702216209658148</v>
       </c>
       <c r="C18">
-        <v>0.18794090417335127</v>
+        <v>0.20053095095819762</v>
       </c>
       <c r="D18">
-        <v>0.46422552969655684</v>
+        <v>0.44906847625775009</v>
       </c>
       <c r="E18">
-        <v>0.94273502981403401</v>
+        <v>0.93934631538536573</v>
       </c>
     </row>
     <row r="19">
@@ -1637,16 +1637,16 @@
         <v>87</v>
       </c>
       <c r="B19">
-        <v>0.65976071460772967</v>
+        <v>0.65990316316536268</v>
       </c>
       <c r="C19">
-        <v>0.61335628927590491</v>
+        <v>0.61395412342376854</v>
       </c>
       <c r="D19">
-        <v>0.43222507541203486</v>
+        <v>0.41740737239365239</v>
       </c>
       <c r="E19">
-        <v>0.93533353035476741</v>
+        <v>0.93156703162849719</v>
       </c>
     </row>
     <row r="20">
@@ -1654,16 +1654,16 @@
         <v>88</v>
       </c>
       <c r="B20">
-        <v>0.61033157636876678</v>
+        <v>0.60744512371337112</v>
       </c>
       <c r="C20">
-        <v>0.55488810277002099</v>
+        <v>0.55265868503004423</v>
       </c>
       <c r="D20">
-        <v>0.43672983408746191</v>
+        <v>0.42206164892062714</v>
       </c>
       <c r="E20">
-        <v>0.93643364671490026</v>
+        <v>0.93277527302164553</v>
       </c>
     </row>
     <row r="21">
@@ -1671,16 +1671,16 @@
         <v>89</v>
       </c>
       <c r="B21">
-        <v>0.74332002454423496</v>
+        <v>0.74400183617474536</v>
       </c>
       <c r="C21">
-        <v>0.70281443410571387</v>
+        <v>0.70473948744544235</v>
       </c>
       <c r="D21">
-        <v>0.42658145967339672</v>
+        <v>0.41125401993791555</v>
       </c>
       <c r="E21">
-        <v>0.93392628118674414</v>
+        <v>0.9299326497986401</v>
       </c>
     </row>
     <row r="22">
@@ -1688,16 +1688,16 @@
         <v>90</v>
       </c>
       <c r="B22">
-        <v>0.75955882160231458</v>
+        <v>0.75865434474670312</v>
       </c>
       <c r="C22">
-        <v>0.724805030149963</v>
+        <v>0.72375332757437916</v>
       </c>
       <c r="D22">
-        <v>0.42606529162018753</v>
+        <v>0.41098419044898116</v>
       </c>
       <c r="E22">
-        <v>0.93379592730747929</v>
+        <v>0.92985999411442655</v>
       </c>
     </row>
     <row r="23">
@@ -1705,16 +1705,16 @@
         <v>91</v>
       </c>
       <c r="B23">
-        <v>0.67642171967914766</v>
+        <v>0.6762775285988154</v>
       </c>
       <c r="C23">
-        <v>0.62971163322889856</v>
+        <v>0.63007304074528725</v>
       </c>
       <c r="D23">
-        <v>0.43162552827468886</v>
+        <v>0.41651398454986593</v>
       </c>
       <c r="E23">
-        <v>0.93518557967801208</v>
+        <v>0.93133238433475152</v>
       </c>
     </row>
     <row r="24">
@@ -1722,16 +1722,16 @@
         <v>92</v>
       </c>
       <c r="B24">
-        <v>0.69513450010582534</v>
+        <v>0.69386827898254022</v>
       </c>
       <c r="C24">
-        <v>0.64966957057701935</v>
+        <v>0.64837663663662637</v>
       </c>
       <c r="D24">
-        <v>0.43047783149984775</v>
+        <v>0.41536514361429455</v>
       </c>
       <c r="E24">
-        <v>0.93490134358069532</v>
+        <v>0.93102933402395294</v>
       </c>
     </row>
   </sheetData>
@@ -1753,7 +1753,7 @@
         <v>94</v>
       </c>
       <c r="B2">
-        <v>0.89980548376827996</v>
+        <v>0.89085471361440993</v>
       </c>
     </row>
     <row r="4">
@@ -1778,16 +1778,16 @@
         <v>100</v>
       </c>
       <c r="B5">
-        <v>0.60765057404749367</v>
+        <v>0.60819780597281548</v>
       </c>
       <c r="C5">
-        <v>0.54099130370298742</v>
+        <v>0.53935298750473015</v>
       </c>
       <c r="D5">
-        <v>0.34711186131012206</v>
+        <v>0.3238364661916715</v>
       </c>
       <c r="E5">
-        <v>0.89480876128231535</v>
+        <v>0.88456541029362779</v>
       </c>
     </row>
     <row r="6">
@@ -1795,16 +1795,16 @@
         <v>101</v>
       </c>
       <c r="B6">
-        <v>0.57890901691872954</v>
+        <v>0.57778376077879723</v>
       </c>
       <c r="C6">
-        <v>0.50613589588786334</v>
+        <v>0.50276421382225001</v>
       </c>
       <c r="D6">
-        <v>0.34931225267703742</v>
+        <v>0.32606512477130556</v>
       </c>
       <c r="E6">
-        <v>0.89571783295340035</v>
+        <v>0.88559879118161744</v>
       </c>
     </row>
     <row r="7">
@@ -1812,16 +1812,16 @@
         <v>102</v>
       </c>
       <c r="B7">
-        <v>0.5704209036028508</v>
+        <v>0.56995610225589366</v>
       </c>
       <c r="C7">
-        <v>0.50065923643525823</v>
+        <v>0.49766811609716827</v>
       </c>
       <c r="D7">
-        <v>0.34918428976873922</v>
+        <v>0.32638993295791435</v>
       </c>
       <c r="E7">
-        <v>0.89566522970794993</v>
+        <v>0.88574841932256598</v>
       </c>
     </row>
     <row r="8">
@@ -1829,16 +1829,16 @@
         <v>103</v>
       </c>
       <c r="B8">
-        <v>0.53503182891015633</v>
+        <v>0.53645401598006992</v>
       </c>
       <c r="C8">
-        <v>0.45733791410152069</v>
+        <v>0.45654114235215276</v>
       </c>
       <c r="D8">
-        <v>0.35260948418173588</v>
+        <v>0.32961501160310597</v>
       </c>
       <c r="E8">
-        <v>0.89706219246221153</v>
+        <v>0.88722079518052255</v>
       </c>
     </row>
     <row r="9">
@@ -1846,16 +1846,16 @@
         <v>104</v>
       </c>
       <c r="B9">
-        <v>0.54932073727996222</v>
+        <v>0.54773926891713187</v>
       </c>
       <c r="C9">
-        <v>0.47584282472940015</v>
+        <v>0.47202409141936263</v>
       </c>
       <c r="D9">
-        <v>0.35127111453286131</v>
+        <v>0.32849871559948751</v>
       </c>
       <c r="E9">
-        <v>0.89651906501406109</v>
+        <v>0.88671388157372577</v>
       </c>
     </row>
     <row r="10">
@@ -1863,16 +1863,16 @@
         <v>105</v>
       </c>
       <c r="B10">
-        <v>0.76272895271912244</v>
+        <v>0.72941299464206544</v>
       </c>
       <c r="C10">
-        <v>0.7117936217212274</v>
+        <v>0.67393034620805248</v>
       </c>
       <c r="D10">
-        <v>0.33088834881486806</v>
+        <v>0.31310874268859251</v>
       </c>
       <c r="E10">
-        <v>0.88779554608734645</v>
+        <v>0.87942149660198099</v>
       </c>
     </row>
     <row r="11">
@@ -1880,16 +1880,16 @@
         <v>106</v>
       </c>
       <c r="B11">
-        <v>0.79083360931839053</v>
+        <v>0.7555214115293436</v>
       </c>
       <c r="C11">
-        <v>0.74635828466019827</v>
+        <v>0.70509800240443421</v>
       </c>
       <c r="D11">
-        <v>0.3283942465983597</v>
+        <v>0.31079282300349548</v>
       </c>
       <c r="E11">
-        <v>0.88666629527227803</v>
+        <v>0.87827264543474437</v>
       </c>
     </row>
     <row r="12">
@@ -1897,16 +1897,16 @@
         <v>107</v>
       </c>
       <c r="B12">
-        <v>0.74898648072644181</v>
+        <v>0.71592779032245291</v>
       </c>
       <c r="C12">
-        <v>0.69562621214810938</v>
+        <v>0.659755437365384</v>
       </c>
       <c r="D12">
-        <v>0.33254915084140568</v>
+        <v>0.3142985261712421</v>
       </c>
       <c r="E12">
-        <v>0.88853967872568107</v>
+        <v>0.88000627761278505</v>
       </c>
     </row>
     <row r="13">
@@ -1914,16 +1914,16 @@
         <v>108</v>
       </c>
       <c r="B13">
-        <v>0.73765275982885248</v>
+        <v>0.68707030680333925</v>
       </c>
       <c r="C13">
-        <v>0.68385891674021859</v>
+        <v>0.62678762214784201</v>
       </c>
       <c r="D13">
-        <v>0.33440865992823343</v>
+        <v>0.31695771008770446</v>
       </c>
       <c r="E13">
-        <v>0.88936553045657074</v>
+        <v>0.88130015864456968</v>
       </c>
     </row>
     <row r="14">
@@ -1931,16 +1931,16 @@
         <v>109</v>
       </c>
       <c r="B14">
-        <v>0.77405707165228466</v>
+        <v>0.74111284797246979</v>
       </c>
       <c r="C14">
-        <v>0.72439603017699539</v>
+        <v>0.68819618466642296</v>
       </c>
       <c r="D14">
-        <v>0.32982355817976178</v>
+        <v>0.31204809528848637</v>
       </c>
       <c r="E14">
-        <v>0.8873151804133691</v>
+        <v>0.8788970884648748</v>
       </c>
     </row>
     <row r="15">
@@ -1948,16 +1948,16 @@
         <v>110</v>
       </c>
       <c r="B15">
-        <v>0.7321382045732433</v>
+        <v>0.68861765846443657</v>
       </c>
       <c r="C15">
-        <v>0.6767540676300533</v>
+        <v>0.62798229627429736</v>
       </c>
       <c r="D15">
-        <v>0.33478932057131988</v>
+        <v>0.31689179019138158</v>
       </c>
       <c r="E15">
-        <v>0.88953364742748453</v>
+        <v>0.88126830081228347</v>
       </c>
     </row>
     <row r="16">
@@ -1965,16 +1965,16 @@
         <v>111</v>
       </c>
       <c r="B16">
-        <v>0.44061752009594934</v>
+        <v>0.44039033537765104</v>
       </c>
       <c r="C16">
-        <v>0.34975492578928696</v>
+        <v>0.35068942179869245</v>
       </c>
       <c r="D16">
-        <v>0.36286363371859487</v>
+        <v>0.33943492711405776</v>
       </c>
       <c r="E16">
-        <v>0.90111114928563685</v>
+        <v>0.89155996381164715</v>
       </c>
     </row>
     <row r="17">
@@ -1982,16 +1982,16 @@
         <v>112</v>
       </c>
       <c r="B17">
-        <v>0.47620613915187499</v>
+        <v>0.46516125289689464</v>
       </c>
       <c r="C17">
-        <v>0.38898181168285684</v>
+        <v>0.37744053680909989</v>
       </c>
       <c r="D17">
-        <v>0.35988615307866706</v>
+        <v>0.33712299320784628</v>
       </c>
       <c r="E17">
-        <v>0.89995551667692608</v>
+        <v>0.89055737468229412</v>
       </c>
     </row>
     <row r="18">
@@ -1999,16 +1999,16 @@
         <v>113</v>
       </c>
       <c r="B18">
-        <v>0.55467051167483483</v>
+        <v>0.5547657433496157</v>
       </c>
       <c r="C18">
-        <v>0.47558276939538946</v>
+        <v>0.47615009455247082</v>
       </c>
       <c r="D18">
-        <v>0.35284101886260411</v>
+        <v>0.32930500997207696</v>
       </c>
       <c r="E18">
-        <v>0.89715580056323885</v>
+        <v>0.88708030908991553</v>
       </c>
     </row>
     <row r="19">
@@ -2016,16 +2016,16 @@
         <v>114</v>
       </c>
       <c r="B19">
-        <v>0.52646442951524608</v>
+        <v>0.50651347460288754</v>
       </c>
       <c r="C19">
-        <v>0.44420698421811888</v>
+        <v>0.42256245024194994</v>
       </c>
       <c r="D19">
-        <v>0.35552601201254852</v>
+        <v>0.33320641973330223</v>
       </c>
       <c r="E19">
-        <v>0.89823382852846245</v>
+        <v>0.88883246494201507</v>
       </c>
     </row>
     <row r="20">
@@ -2033,16 +2033,16 @@
         <v>115</v>
       </c>
       <c r="B20">
-        <v>0.49350866726822967</v>
+        <v>0.49238339463829822</v>
       </c>
       <c r="C20">
-        <v>0.40812797146854823</v>
+        <v>0.40741265810670729</v>
       </c>
       <c r="D20">
-        <v>0.35838494836191814</v>
+        <v>0.33493932461821685</v>
       </c>
       <c r="E20">
-        <v>0.89936672332607048</v>
+        <v>0.8895998084666662</v>
       </c>
     </row>
     <row r="21">
@@ -2050,16 +2050,16 @@
         <v>116</v>
       </c>
       <c r="B21">
-        <v>0.64001003189013472</v>
+        <v>0.63608330714518779</v>
       </c>
       <c r="C21">
-        <v>0.57090761410195578</v>
+        <v>0.56675496613262022</v>
       </c>
       <c r="D21">
-        <v>0.34507033591622038</v>
+        <v>0.32179368951610843</v>
       </c>
       <c r="E21">
-        <v>0.8939566341337134</v>
+        <v>0.88360780369828562</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2081,7 @@
         <v>118</v>
       </c>
       <c r="B2">
-        <v>0.66211117647631301</v>
+        <v>0.65623927279165772</v>
       </c>
     </row>
     <row r="4">
@@ -2106,16 +2106,16 @@
         <v>124</v>
       </c>
       <c r="B5">
-        <v>0.72440688132534969</v>
+        <v>0.72343446334671924</v>
       </c>
       <c r="C5">
-        <v>0.45125479042373434</v>
+        <v>0.45186009875595773</v>
       </c>
       <c r="D5">
-        <v>0.31803270388592036</v>
+        <v>0.30679225020535938</v>
       </c>
       <c r="E5">
-        <v>0.58316623964145087</v>
+        <v>0.57039265708229547</v>
       </c>
     </row>
     <row r="6">
@@ -2123,16 +2123,16 @@
         <v>125</v>
       </c>
       <c r="B6">
-        <v>0.64920938872831568</v>
+        <v>0.6483559048496802</v>
       </c>
       <c r="C6">
-        <v>0.34990273077469564</v>
+        <v>0.34956194140277003</v>
       </c>
       <c r="D6">
-        <v>0.38755529935631444</v>
+        <v>0.37960635378077401</v>
       </c>
       <c r="E6">
-        <v>0.65498222979015974</v>
+        <v>0.64734585900123698</v>
       </c>
     </row>
     <row r="7">
@@ -2140,16 +2140,16 @@
         <v>126</v>
       </c>
       <c r="B7">
-        <v>0.76412230331561881</v>
+        <v>0.74150754987620371</v>
       </c>
       <c r="C7">
-        <v>0.46341058296824783</v>
+        <v>0.45718989533615068</v>
       </c>
       <c r="D7">
-        <v>0.29898614071388335</v>
+        <v>0.298158036314709</v>
       </c>
       <c r="E7">
-        <v>0.56131037600992029</v>
+        <v>0.56033646737063059</v>
       </c>
     </row>
     <row r="8">
@@ -2157,16 +2157,16 @@
         <v>127</v>
       </c>
       <c r="B8">
-        <v>0.74125341506934572</v>
+        <v>0.72253835183014314</v>
       </c>
       <c r="C8">
-        <v>0.46009249225466198</v>
+        <v>0.45330117956787463</v>
       </c>
       <c r="D8">
-        <v>0.30776620003126054</v>
+        <v>0.30698763860471773</v>
       </c>
       <c r="E8">
-        <v>0.57151351471381817</v>
+        <v>0.57061773424838258</v>
       </c>
     </row>
   </sheetData>
@@ -2188,7 +2188,7 @@
         <v>129</v>
       </c>
       <c r="B2">
-        <v>0.94879129730325307</v>
+        <v>0.9534737653335531</v>
       </c>
     </row>
     <row r="4">
@@ -2213,16 +2213,16 @@
         <v>135</v>
       </c>
       <c r="B5">
-        <v>0.93251077638388924</v>
+        <v>0.9400258716737856</v>
       </c>
       <c r="C5">
-        <v>0.87853374268790541</v>
+        <v>0.89202801180388513</v>
       </c>
       <c r="D5">
-        <v>0.82029816548400292</v>
+        <v>0.83224411654333985</v>
       </c>
       <c r="E5">
-        <v>0.93194649541525321</v>
+        <v>0.93704011097758799</v>
       </c>
     </row>
     <row r="6">
@@ -2230,16 +2230,16 @@
         <v>136</v>
       </c>
       <c r="B6">
-        <v>0.87021774315021971</v>
+        <v>0.88296490018819718</v>
       </c>
       <c r="C6">
-        <v>0.77377575858429226</v>
+        <v>0.79537574322487448</v>
       </c>
       <c r="D6">
-        <v>0.89889402367670834</v>
+        <v>0.90487469804358511</v>
       </c>
       <c r="E6">
-        <v>0.96386217447067379</v>
+        <v>0.96614456004906146</v>
       </c>
     </row>
     <row r="7">
@@ -2247,16 +2247,16 @@
         <v>137</v>
       </c>
       <c r="B7">
-        <v>0.96807253793751136</v>
+        <v>0.96712286367211653</v>
       </c>
       <c r="C7">
-        <v>0.94150521098901219</v>
+        <v>0.94006630972687655</v>
       </c>
       <c r="D7">
-        <v>0.77628584993049388</v>
+        <v>0.79860742705905385</v>
       </c>
       <c r="E7">
-        <v>0.91235734922482714</v>
+        <v>0.92245825461007924</v>
       </c>
     </row>
     <row r="8">
@@ -2264,16 +2264,16 @@
         <v>138</v>
       </c>
       <c r="B8">
-        <v>0.95472308681019069</v>
+        <v>0.95834418544591693</v>
       </c>
       <c r="C8">
-        <v>0.9170570109632542</v>
+        <v>0.92380541615946565</v>
       </c>
       <c r="D8">
-        <v>0.79430254063074579</v>
+        <v>0.81104528041326462</v>
       </c>
       <c r="E8">
-        <v>0.92053733462154352</v>
+        <v>0.9279373785140459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>